<commit_message>
Still exploring a few possibilities
</commit_message>
<xml_diff>
--- a/data/data_diet_Agazella.xlsx
+++ b/data/data_diet_Agazella.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0879F40-D0E5-4C06-AF35-12424567BD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C053964C-61F2-46A4-B404-B534434AD9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -889,11 +889,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M491"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39:I98"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
@@ -5113,7 +5113,7 @@
         <v>86</v>
       </c>
       <c r="J126">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K126" t="s">
         <v>93</v>
@@ -5143,7 +5143,7 @@
         <v>86</v>
       </c>
       <c r="J127">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K127" t="s">
         <v>93</v>
@@ -5169,7 +5169,7 @@
         <v>86</v>
       </c>
       <c r="J128">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K128" t="s">
         <v>93</v>
@@ -5199,7 +5199,7 @@
         <v>86</v>
       </c>
       <c r="J129">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K129" t="s">
         <v>93</v>
@@ -5229,7 +5229,7 @@
         <v>86</v>
       </c>
       <c r="J130">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K130" t="s">
         <v>93</v>
@@ -5259,7 +5259,7 @@
         <v>86</v>
       </c>
       <c r="J131">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K131" t="s">
         <v>93</v>
@@ -5282,7 +5282,7 @@
         <v>86</v>
       </c>
       <c r="J132">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K132" t="s">
         <v>93</v>
@@ -5312,7 +5312,7 @@
         <v>86</v>
       </c>
       <c r="J133">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K133" t="s">
         <v>93</v>
@@ -5342,7 +5342,7 @@
         <v>86</v>
       </c>
       <c r="J134">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K134" t="s">
         <v>93</v>
@@ -5372,7 +5372,7 @@
         <v>86</v>
       </c>
       <c r="J135">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K135" t="s">
         <v>93</v>
@@ -5402,7 +5402,7 @@
         <v>86</v>
       </c>
       <c r="J136">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K136" t="s">
         <v>93</v>
@@ -5432,7 +5432,7 @@
         <v>86</v>
       </c>
       <c r="J137">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K137" t="s">
         <v>93</v>
@@ -5462,7 +5462,7 @@
         <v>86</v>
       </c>
       <c r="J138">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K138" t="s">
         <v>93</v>
@@ -5491,7 +5491,7 @@
         <v>86</v>
       </c>
       <c r="J139">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K139" t="s">
         <v>93</v>
@@ -5520,7 +5520,7 @@
         <v>86</v>
       </c>
       <c r="J140">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K140" t="s">
         <v>93</v>
@@ -5549,7 +5549,7 @@
         <v>86</v>
       </c>
       <c r="J141">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K141" t="s">
         <v>93</v>
@@ -5572,7 +5572,7 @@
         <v>86</v>
       </c>
       <c r="J142">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K142" t="s">
         <v>93</v>
@@ -5602,7 +5602,7 @@
         <v>86</v>
       </c>
       <c r="J143">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K143" t="s">
         <v>93</v>
@@ -5631,7 +5631,7 @@
         <v>86</v>
       </c>
       <c r="J144">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K144" t="s">
         <v>93</v>
@@ -5660,7 +5660,7 @@
         <v>86</v>
       </c>
       <c r="J145">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="K145" t="s">
         <v>93</v>
@@ -5690,7 +5690,7 @@
         <v>86</v>
       </c>
       <c r="J146">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K146" t="s">
         <v>93</v>
@@ -5720,7 +5720,7 @@
         <v>86</v>
       </c>
       <c r="J147">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K147" t="s">
         <v>93</v>
@@ -5746,7 +5746,7 @@
         <v>86</v>
       </c>
       <c r="J148">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K148" t="s">
         <v>93</v>
@@ -5776,7 +5776,7 @@
         <v>86</v>
       </c>
       <c r="J149">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K149" t="s">
         <v>93</v>
@@ -5806,7 +5806,7 @@
         <v>86</v>
       </c>
       <c r="J150">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K150" t="s">
         <v>93</v>
@@ -5836,7 +5836,7 @@
         <v>86</v>
       </c>
       <c r="J151">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K151" t="s">
         <v>93</v>
@@ -5859,7 +5859,7 @@
         <v>86</v>
       </c>
       <c r="J152">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K152" t="s">
         <v>93</v>
@@ -5889,7 +5889,7 @@
         <v>86</v>
       </c>
       <c r="J153">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K153" t="s">
         <v>93</v>
@@ -5919,7 +5919,7 @@
         <v>86</v>
       </c>
       <c r="J154">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K154" t="s">
         <v>93</v>
@@ -5949,7 +5949,7 @@
         <v>86</v>
       </c>
       <c r="J155">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K155" t="s">
         <v>93</v>
@@ -5979,7 +5979,7 @@
         <v>86</v>
       </c>
       <c r="J156">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K156" t="s">
         <v>93</v>
@@ -6009,7 +6009,7 @@
         <v>86</v>
       </c>
       <c r="J157">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K157" t="s">
         <v>93</v>
@@ -6038,7 +6038,7 @@
         <v>86</v>
       </c>
       <c r="J158">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K158" t="s">
         <v>93</v>
@@ -6067,7 +6067,7 @@
         <v>86</v>
       </c>
       <c r="J159">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K159" t="s">
         <v>93</v>
@@ -6096,7 +6096,7 @@
         <v>86</v>
       </c>
       <c r="J160">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="K160" t="s">
         <v>93</v>

</xml_diff>